<commit_message>
Additional material concerning Matroska. Fixed error in utf8.xlsx.
</commit_message>
<xml_diff>
--- a/doc/utf8.xlsx
+++ b/doc/utf8.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="16515" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="16515" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Errors" sheetId="7" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="177">
   <si>
     <t>S</t>
   </si>
@@ -1044,6 +1044,9 @@
   </si>
   <si>
     <t>See http://www.whatwg.org/specs/web-apps/current-work/multipage/infrastructure.html#utf-8</t>
+  </si>
+  <si>
+    <t>One byte in the range C0 to FD that is not followed by a byte in the range 80 to BF</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1152,31 +1155,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1480,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1491,10 +1495,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="17"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
@@ -1566,8 +1570,8 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>166</v>
+      <c r="C11" s="16" t="s">
+        <v>176</v>
       </c>
       <c r="D11" t="s">
         <v>168</v>
@@ -1650,7 +1654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
@@ -1678,28 +1682,28 @@
       <c r="I2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
       <c r="M2" s="8" t="s">
         <v>61</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21" t="s">
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
       <c r="V2" s="8" t="s">
         <v>65</v>
       </c>
@@ -1789,11 +1793,11 @@
       <c r="I9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
       <c r="M9" s="8" t="s">
         <v>121</v>
       </c>
@@ -1844,11 +1848,11 @@
       <c r="I10" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
       <c r="M10" s="18" t="s">
         <v>44</v>
       </c>
@@ -1864,7 +1868,7 @@
       <c r="W10" s="18"/>
       <c r="X10" s="18"/>
       <c r="Y10" s="18"/>
-      <c r="Z10" s="23" t="s">
+      <c r="Z10" s="21" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1891,17 +1895,17 @@
       <c r="W11" s="18"/>
       <c r="X11" s="18"/>
       <c r="Y11" s="18"/>
-      <c r="Z11" s="23"/>
+      <c r="Z11" s="21"/>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="I12" s="18"/>
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="16"/>
+      <c r="K12" s="19"/>
       <c r="L12" s="1" t="s">
         <v>31</v>
       </c>
@@ -1918,7 +1922,7 @@
       <c r="W12" s="18"/>
       <c r="X12" s="18"/>
       <c r="Y12" s="18"/>
-      <c r="Z12" s="23"/>
+      <c r="Z12" s="21"/>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
@@ -1927,11 +1931,11 @@
       <c r="I13" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="J13" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
       <c r="M13" s="18" t="s">
         <v>55</v>
       </c>
@@ -1987,26 +1991,26 @@
       <c r="I15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="21" t="s">
+      <c r="J15" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="16" t="s">
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
-      <c r="U15" s="16"/>
-      <c r="V15" s="16"/>
-      <c r="W15" s="16"/>
-      <c r="X15" s="16"/>
-      <c r="Y15" s="16"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
       <c r="Z15" s="14" t="s">
         <v>128</v>
       </c>
@@ -2049,28 +2053,28 @@
       <c r="I17" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J17" s="21" t="s">
+      <c r="J17" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="21"/>
+      <c r="K17" s="20"/>
       <c r="L17" t="s">
         <v>57</v>
       </c>
-      <c r="M17" s="16" t="s">
+      <c r="M17" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16"/>
-      <c r="V17" s="16"/>
-      <c r="W17" s="16"/>
-      <c r="X17" s="16"/>
-      <c r="Y17" s="16"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="19"/>
       <c r="Z17" s="14" t="s">
         <v>128</v>
       </c>
@@ -2113,11 +2117,11 @@
       <c r="I19" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
       <c r="M19" s="18" t="s">
         <v>55</v>
       </c>
@@ -2144,26 +2148,26 @@
       <c r="I20" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="21" t="s">
+      <c r="J20" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="16" t="s">
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
-      <c r="T20" s="16"/>
-      <c r="U20" s="16"/>
-      <c r="V20" s="16"/>
-      <c r="W20" s="16"/>
-      <c r="X20" s="16"/>
-      <c r="Y20" s="16"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="19"/>
+      <c r="X20" s="19"/>
+      <c r="Y20" s="19"/>
       <c r="Z20" s="14" t="s">
         <v>128</v>
       </c>
@@ -2209,25 +2213,25 @@
       <c r="J22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K22" s="21" t="s">
+      <c r="K22" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="L22" s="21"/>
-      <c r="M22" s="16" t="s">
+      <c r="L22" s="20"/>
+      <c r="M22" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="16"/>
-      <c r="S22" s="16"/>
-      <c r="T22" s="16"/>
-      <c r="U22" s="16"/>
-      <c r="V22" s="16"/>
-      <c r="W22" s="16"/>
-      <c r="X22" s="16"/>
-      <c r="Y22" s="16"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="19"/>
+      <c r="W22" s="19"/>
+      <c r="X22" s="19"/>
+      <c r="Y22" s="19"/>
       <c r="Z22" s="14" t="s">
         <v>128</v>
       </c>
@@ -2239,11 +2243,11 @@
       <c r="I23" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="J23" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
       <c r="M23" s="18" t="s">
         <v>55</v>
       </c>
@@ -2271,26 +2275,26 @@
       <c r="I24" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J24" s="16" t="s">
+      <c r="J24" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16" t="s">
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="16"/>
-      <c r="T24" s="16"/>
-      <c r="U24" s="16"/>
-      <c r="V24" s="16"/>
-      <c r="W24" s="16"/>
-      <c r="X24" s="16"/>
-      <c r="Y24" s="16"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="19"/>
+      <c r="W24" s="19"/>
+      <c r="X24" s="19"/>
+      <c r="Y24" s="19"/>
       <c r="Z24" s="10" t="s">
         <v>132</v>
       </c>
@@ -2302,11 +2306,11 @@
       <c r="I25" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J25" s="21" t="s">
+      <c r="J25" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
       <c r="M25" s="18" t="s">
         <v>55</v>
       </c>
@@ -2338,21 +2342,21 @@
       </c>
       <c r="K26" s="22"/>
       <c r="L26" s="22"/>
-      <c r="M26" s="16" t="s">
+      <c r="M26" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="16"/>
-      <c r="T26" s="16"/>
-      <c r="U26" s="16"/>
-      <c r="V26" s="16"/>
-      <c r="W26" s="16"/>
-      <c r="X26" s="16"/>
-      <c r="Y26" s="16"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="19"/>
+      <c r="W26" s="19"/>
+      <c r="X26" s="19"/>
+      <c r="Y26" s="19"/>
       <c r="Z26" s="10" t="s">
         <v>132</v>
       </c>
@@ -2364,26 +2368,26 @@
       <c r="I27" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J27" s="21" t="s">
+      <c r="J27" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="16" t="s">
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="16"/>
-      <c r="S27" s="16"/>
-      <c r="T27" s="16"/>
-      <c r="U27" s="16"/>
-      <c r="V27" s="16"/>
-      <c r="W27" s="16"/>
-      <c r="X27" s="16"/>
-      <c r="Y27" s="16"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="19"/>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="19"/>
       <c r="Z27" s="14" t="s">
         <v>128</v>
       </c>
@@ -2395,11 +2399,11 @@
       <c r="I28" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J28" s="21" t="s">
+      <c r="J28" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
       <c r="M28" s="18" t="s">
         <v>55</v>
       </c>
@@ -2431,21 +2435,21 @@
       </c>
       <c r="K29" s="22"/>
       <c r="L29" s="22"/>
-      <c r="M29" s="16" t="s">
+      <c r="M29" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16"/>
-      <c r="W29" s="16"/>
-      <c r="X29" s="16"/>
-      <c r="Y29" s="16"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="19"/>
+      <c r="Y29" s="19"/>
       <c r="Z29" s="10" t="s">
         <v>132</v>
       </c>
@@ -2460,25 +2464,25 @@
       <c r="J30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K30" s="17" t="s">
+      <c r="K30" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="L30" s="17"/>
-      <c r="M30" s="16" t="s">
+      <c r="L30" s="25"/>
+      <c r="M30" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="16"/>
-      <c r="T30" s="16"/>
-      <c r="U30" s="16"/>
-      <c r="V30" s="16"/>
-      <c r="W30" s="16"/>
-      <c r="X30" s="16"/>
-      <c r="Y30" s="16"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="19"/>
+      <c r="X30" s="19"/>
+      <c r="Y30" s="19"/>
       <c r="Z30" s="14" t="s">
         <v>128</v>
       </c>
@@ -2490,11 +2494,11 @@
       <c r="I31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J31" s="21" t="s">
+      <c r="J31" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
       <c r="M31" s="18" t="s">
         <v>55</v>
       </c>
@@ -2526,21 +2530,21 @@
       </c>
       <c r="K32" s="22"/>
       <c r="L32" s="22"/>
-      <c r="M32" s="16" t="s">
+      <c r="M32" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="16"/>
-      <c r="T32" s="16"/>
-      <c r="U32" s="16"/>
-      <c r="V32" s="16"/>
-      <c r="W32" s="16"/>
-      <c r="X32" s="16"/>
-      <c r="Y32" s="16"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="19"/>
+      <c r="X32" s="19"/>
+      <c r="Y32" s="19"/>
       <c r="Z32" s="10" t="s">
         <v>132</v>
       </c>
@@ -2552,11 +2556,11 @@
       <c r="I33" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="J33" s="17" t="s">
+      <c r="J33" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
       <c r="M33" s="18" t="s">
         <v>55</v>
       </c>
@@ -2584,26 +2588,26 @@
       <c r="I34" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="J34" s="19" t="s">
+      <c r="J34" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="16" t="s">
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="N34" s="16"/>
-      <c r="O34" s="16"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="16"/>
-      <c r="S34" s="16"/>
-      <c r="T34" s="16"/>
-      <c r="U34" s="16"/>
-      <c r="V34" s="16"/>
-      <c r="W34" s="16"/>
-      <c r="X34" s="16"/>
-      <c r="Y34" s="16"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19"/>
+      <c r="X34" s="19"/>
+      <c r="Y34" s="19"/>
       <c r="Z34" s="10" t="s">
         <v>132</v>
       </c>
@@ -2619,26 +2623,26 @@
       <c r="I35" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J35" s="20" t="s">
+      <c r="J35" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="16" t="s">
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="N35" s="16"/>
-      <c r="O35" s="16"/>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="16"/>
-      <c r="R35" s="16"/>
-      <c r="S35" s="16"/>
-      <c r="T35" s="16"/>
-      <c r="U35" s="16"/>
-      <c r="V35" s="16"/>
-      <c r="W35" s="16"/>
-      <c r="X35" s="16"/>
-      <c r="Y35" s="16"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+      <c r="V35" s="19"/>
+      <c r="W35" s="19"/>
+      <c r="X35" s="19"/>
+      <c r="Y35" s="19"/>
       <c r="Z35" s="14" t="s">
         <v>128</v>
       </c>
@@ -2654,11 +2658,11 @@
       <c r="I36" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J36" s="20" t="s">
+      <c r="J36" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
       <c r="M36" s="18" t="s">
         <v>55</v>
       </c>
@@ -2689,26 +2693,26 @@
       <c r="I37" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J37" s="16" t="s">
+      <c r="J37" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="K37" s="16"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="16" t="s">
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="N37" s="16"/>
-      <c r="O37" s="16"/>
-      <c r="P37" s="16"/>
-      <c r="Q37" s="16"/>
-      <c r="R37" s="16"/>
-      <c r="S37" s="16"/>
-      <c r="T37" s="16"/>
-      <c r="U37" s="16"/>
-      <c r="V37" s="16"/>
-      <c r="W37" s="16"/>
-      <c r="X37" s="16"/>
-      <c r="Y37" s="16"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
+      <c r="U37" s="19"/>
+      <c r="V37" s="19"/>
+      <c r="W37" s="19"/>
+      <c r="X37" s="19"/>
+      <c r="Y37" s="19"/>
       <c r="Z37" s="10" t="s">
         <v>132</v>
       </c>
@@ -2724,26 +2728,26 @@
       <c r="I38" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J38" s="20" t="s">
+      <c r="J38" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="16" t="s">
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="N38" s="16"/>
-      <c r="O38" s="16"/>
-      <c r="P38" s="16"/>
-      <c r="Q38" s="16"/>
-      <c r="R38" s="16"/>
-      <c r="S38" s="16"/>
-      <c r="T38" s="16"/>
-      <c r="U38" s="16"/>
-      <c r="V38" s="16"/>
-      <c r="W38" s="16"/>
-      <c r="X38" s="16"/>
-      <c r="Y38" s="16"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="19"/>
+      <c r="X38" s="19"/>
+      <c r="Y38" s="19"/>
       <c r="Z38" s="14" t="s">
         <v>128</v>
       </c>
@@ -2759,11 +2763,11 @@
       <c r="I39" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J39" s="20" t="s">
+      <c r="J39" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
       <c r="M39" s="18" t="s">
         <v>55</v>
       </c>
@@ -2794,26 +2798,26 @@
       <c r="I40" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J40" s="20" t="s">
+      <c r="J40" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="16" t="s">
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="N40" s="16"/>
-      <c r="O40" s="16"/>
-      <c r="P40" s="16"/>
-      <c r="Q40" s="16"/>
-      <c r="R40" s="16"/>
-      <c r="S40" s="16"/>
-      <c r="T40" s="16"/>
-      <c r="U40" s="16"/>
-      <c r="V40" s="16"/>
-      <c r="W40" s="16"/>
-      <c r="X40" s="16"/>
-      <c r="Y40" s="16"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
+      <c r="Y40" s="19"/>
       <c r="Z40" s="10" t="s">
         <v>132</v>
       </c>
@@ -2829,26 +2833,26 @@
       <c r="I41" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="J41" s="16" t="s">
+      <c r="J41" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="K41" s="16"/>
-      <c r="L41" s="16"/>
-      <c r="M41" s="16" t="s">
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="N41" s="16"/>
-      <c r="O41" s="16"/>
-      <c r="P41" s="16"/>
-      <c r="Q41" s="16"/>
-      <c r="R41" s="16"/>
-      <c r="S41" s="16"/>
-      <c r="T41" s="16"/>
-      <c r="U41" s="16"/>
-      <c r="V41" s="16"/>
-      <c r="W41" s="16"/>
-      <c r="X41" s="16"/>
-      <c r="Y41" s="16"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="19"/>
+      <c r="T41" s="19"/>
+      <c r="U41" s="19"/>
+      <c r="V41" s="19"/>
+      <c r="W41" s="19"/>
+      <c r="X41" s="19"/>
+      <c r="Y41" s="19"/>
       <c r="Z41" s="10" t="s">
         <v>131</v>
       </c>
@@ -2864,26 +2868,26 @@
       <c r="I42" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J42" s="20" t="s">
+      <c r="J42" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="16" t="s">
+      <c r="K42" s="23"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="N42" s="16"/>
-      <c r="O42" s="16"/>
-      <c r="P42" s="16"/>
-      <c r="Q42" s="16"/>
-      <c r="R42" s="16"/>
-      <c r="S42" s="16"/>
-      <c r="T42" s="16"/>
-      <c r="U42" s="16"/>
-      <c r="V42" s="16"/>
-      <c r="W42" s="16"/>
-      <c r="X42" s="16"/>
-      <c r="Y42" s="16"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="19"/>
+      <c r="T42" s="19"/>
+      <c r="U42" s="19"/>
+      <c r="V42" s="19"/>
+      <c r="W42" s="19"/>
+      <c r="X42" s="19"/>
+      <c r="Y42" s="19"/>
       <c r="Z42" s="14" t="s">
         <v>128</v>
       </c>
@@ -2899,11 +2903,11 @@
       <c r="I43" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J43" s="20" t="s">
+      <c r="J43" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="23"/>
       <c r="M43" s="18" t="s">
         <v>55</v>
       </c>
@@ -2934,26 +2938,26 @@
       <c r="I44" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J44" s="20" t="s">
+      <c r="J44" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
-      <c r="M44" s="16" t="s">
+      <c r="K44" s="23"/>
+      <c r="L44" s="23"/>
+      <c r="M44" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="N44" s="16"/>
-      <c r="O44" s="16"/>
-      <c r="P44" s="16"/>
-      <c r="Q44" s="16"/>
-      <c r="R44" s="16"/>
-      <c r="S44" s="16"/>
-      <c r="T44" s="16"/>
-      <c r="U44" s="16"/>
-      <c r="V44" s="16"/>
-      <c r="W44" s="16"/>
-      <c r="X44" s="16"/>
-      <c r="Y44" s="16"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="19"/>
+      <c r="T44" s="19"/>
+      <c r="U44" s="19"/>
+      <c r="V44" s="19"/>
+      <c r="W44" s="19"/>
+      <c r="X44" s="19"/>
+      <c r="Y44" s="19"/>
       <c r="Z44" s="10" t="s">
         <v>132</v>
       </c>
@@ -2969,26 +2973,26 @@
       <c r="I45" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="J45" s="20" t="s">
+      <c r="J45" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
-      <c r="M45" s="16" t="s">
+      <c r="K45" s="23"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="N45" s="16"/>
-      <c r="O45" s="16"/>
-      <c r="P45" s="16"/>
-      <c r="Q45" s="16"/>
-      <c r="R45" s="16"/>
-      <c r="S45" s="16"/>
-      <c r="T45" s="16"/>
-      <c r="U45" s="16"/>
-      <c r="V45" s="16"/>
-      <c r="W45" s="16"/>
-      <c r="X45" s="16"/>
-      <c r="Y45" s="16"/>
+      <c r="N45" s="19"/>
+      <c r="O45" s="19"/>
+      <c r="P45" s="19"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="19"/>
+      <c r="S45" s="19"/>
+      <c r="T45" s="19"/>
+      <c r="U45" s="19"/>
+      <c r="V45" s="19"/>
+      <c r="W45" s="19"/>
+      <c r="X45" s="19"/>
+      <c r="Y45" s="19"/>
       <c r="Z45" s="10" t="s">
         <v>131</v>
       </c>
@@ -3004,49 +3008,73 @@
       <c r="I46" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J46" s="16" t="s">
+      <c r="J46" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="K46" s="16"/>
-      <c r="L46" s="16"/>
-      <c r="M46" s="16" t="s">
+      <c r="K46" s="19"/>
+      <c r="L46" s="19"/>
+      <c r="M46" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="N46" s="16"/>
-      <c r="O46" s="16"/>
-      <c r="P46" s="16"/>
-      <c r="Q46" s="16"/>
-      <c r="R46" s="16"/>
-      <c r="S46" s="16"/>
-      <c r="T46" s="16"/>
-      <c r="U46" s="16"/>
-      <c r="V46" s="16"/>
-      <c r="W46" s="16"/>
-      <c r="X46" s="16"/>
-      <c r="Y46" s="16"/>
+      <c r="N46" s="19"/>
+      <c r="O46" s="19"/>
+      <c r="P46" s="19"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="19"/>
+      <c r="S46" s="19"/>
+      <c r="T46" s="19"/>
+      <c r="U46" s="19"/>
+      <c r="V46" s="19"/>
+      <c r="W46" s="19"/>
+      <c r="X46" s="19"/>
+      <c r="Y46" s="19"/>
       <c r="Z46" s="10" t="s">
         <v>130</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="Z10:Z12"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M13:Y13"/>
-    <mergeCell ref="M14:Y14"/>
-    <mergeCell ref="M10:Y12"/>
-    <mergeCell ref="M15:Y15"/>
-    <mergeCell ref="M17:Y17"/>
-    <mergeCell ref="M20:Y20"/>
-    <mergeCell ref="M22:Y22"/>
+    <mergeCell ref="J46:L46"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="J45:L45"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M33:Y33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="M34:Y34"/>
+    <mergeCell ref="M36:Y36"/>
+    <mergeCell ref="M27:Y27"/>
+    <mergeCell ref="M30:Y30"/>
+    <mergeCell ref="M35:Y35"/>
+    <mergeCell ref="M46:Y46"/>
+    <mergeCell ref="M43:Y43"/>
+    <mergeCell ref="M40:Y40"/>
+    <mergeCell ref="M39:Y39"/>
+    <mergeCell ref="M23:Y23"/>
+    <mergeCell ref="M24:Y24"/>
+    <mergeCell ref="M26:Y26"/>
+    <mergeCell ref="M29:Y29"/>
+    <mergeCell ref="M32:Y32"/>
+    <mergeCell ref="M25:Y25"/>
+    <mergeCell ref="M28:Y28"/>
+    <mergeCell ref="M31:Y31"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="M38:Y38"/>
+    <mergeCell ref="M42:Y42"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="M37:Y37"/>
     <mergeCell ref="J31:L31"/>
     <mergeCell ref="M44:Y44"/>
     <mergeCell ref="M41:Y41"/>
@@ -3063,52 +3091,28 @@
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="J13:L13"/>
-    <mergeCell ref="M38:Y38"/>
-    <mergeCell ref="M42:Y42"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M13:Y13"/>
+    <mergeCell ref="M14:Y14"/>
+    <mergeCell ref="M10:Y12"/>
+    <mergeCell ref="M15:Y15"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="Z10:Z12"/>
+    <mergeCell ref="M17:Y17"/>
+    <mergeCell ref="M20:Y20"/>
+    <mergeCell ref="M22:Y22"/>
     <mergeCell ref="M16:Y16"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="J24:L24"/>
     <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J19:L19"/>
     <mergeCell ref="M18:Y18"/>
     <mergeCell ref="M19:Y19"/>
     <mergeCell ref="M21:Y21"/>
-    <mergeCell ref="M23:Y23"/>
-    <mergeCell ref="M24:Y24"/>
-    <mergeCell ref="M26:Y26"/>
-    <mergeCell ref="M29:Y29"/>
-    <mergeCell ref="M32:Y32"/>
-    <mergeCell ref="M37:Y37"/>
-    <mergeCell ref="M25:Y25"/>
-    <mergeCell ref="M28:Y28"/>
-    <mergeCell ref="M31:Y31"/>
-    <mergeCell ref="M36:Y36"/>
-    <mergeCell ref="M27:Y27"/>
-    <mergeCell ref="M30:Y30"/>
-    <mergeCell ref="M35:Y35"/>
-    <mergeCell ref="M46:Y46"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M33:Y33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="M34:Y34"/>
-    <mergeCell ref="M43:Y43"/>
-    <mergeCell ref="M40:Y40"/>
-    <mergeCell ref="M39:Y39"/>
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="J45:L45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3149,28 +3153,28 @@
       <c r="H2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
       <c r="L2" s="9" t="s">
         <v>61</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21" t="s">
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
       <c r="U2" s="9" t="s">
         <v>65</v>
       </c>
@@ -3260,11 +3264,11 @@
       <c r="H9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
       <c r="L9" s="9" t="s">
         <v>4</v>
       </c>
@@ -3315,11 +3319,11 @@
       <c r="H10" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
       <c r="L10" s="18" t="s">
         <v>78</v>
       </c>
@@ -3335,7 +3339,7 @@
       <c r="V10" s="18"/>
       <c r="W10" s="18"/>
       <c r="X10" s="18"/>
-      <c r="Y10" s="23" t="s">
+      <c r="Y10" s="21" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3362,17 +3366,17 @@
       <c r="V11" s="18"/>
       <c r="W11" s="18"/>
       <c r="X11" s="18"/>
-      <c r="Y11" s="23"/>
+      <c r="Y11" s="21"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="H12" s="18"/>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="J12" s="16"/>
+      <c r="J12" s="19"/>
       <c r="K12" s="2" t="s">
         <v>31</v>
       </c>
@@ -3389,7 +3393,7 @@
       <c r="V12" s="18"/>
       <c r="W12" s="18"/>
       <c r="X12" s="18"/>
-      <c r="Y12" s="23"/>
+      <c r="Y12" s="21"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
@@ -3397,11 +3401,11 @@
       </c>
       <c r="C13" s="6"/>
       <c r="H13" s="18"/>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
       <c r="L13" s="18"/>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
@@ -3415,7 +3419,7 @@
       <c r="V13" s="18"/>
       <c r="W13" s="18"/>
       <c r="X13" s="18"/>
-      <c r="Y13" s="23"/>
+      <c r="Y13" s="21"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -3440,18 +3444,18 @@
       <c r="V14" s="18"/>
       <c r="W14" s="18"/>
       <c r="X14" s="18"/>
-      <c r="Y14" s="23"/>
+      <c r="Y14" s="21"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="H15" s="18"/>
-      <c r="I15" s="21" t="s">
+      <c r="I15" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
       <c r="L15" s="18"/>
       <c r="M15" s="18"/>
       <c r="N15" s="18"/>
@@ -3465,7 +3469,7 @@
       <c r="V15" s="18"/>
       <c r="W15" s="18"/>
       <c r="X15" s="18"/>
-      <c r="Y15" s="23"/>
+      <c r="Y15" s="21"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -3490,17 +3494,17 @@
       <c r="V16" s="18"/>
       <c r="W16" s="18"/>
       <c r="X16" s="18"/>
-      <c r="Y16" s="23"/>
+      <c r="Y16" s="21"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="H17" s="18"/>
-      <c r="I17" s="21" t="s">
+      <c r="I17" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="J17" s="21"/>
+      <c r="J17" s="20"/>
       <c r="K17" s="9" t="s">
         <v>93</v>
       </c>
@@ -3517,7 +3521,7 @@
       <c r="V17" s="18"/>
       <c r="W17" s="18"/>
       <c r="X17" s="18"/>
-      <c r="Y17" s="23"/>
+      <c r="Y17" s="21"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
@@ -3542,7 +3546,7 @@
       <c r="V18" s="18"/>
       <c r="W18" s="18"/>
       <c r="X18" s="18"/>
-      <c r="Y18" s="23"/>
+      <c r="Y18" s="21"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
@@ -3550,11 +3554,11 @@
       </c>
       <c r="C19" s="6"/>
       <c r="H19" s="18"/>
-      <c r="I19" s="19" t="s">
+      <c r="I19" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
       <c r="L19" s="18"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
@@ -3568,18 +3572,18 @@
       <c r="V19" s="18"/>
       <c r="W19" s="18"/>
       <c r="X19" s="18"/>
-      <c r="Y19" s="23"/>
+      <c r="Y19" s="21"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>9</v>
       </c>
       <c r="H20" s="18"/>
-      <c r="I20" s="21" t="s">
+      <c r="I20" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
@@ -3593,7 +3597,7 @@
       <c r="V20" s="18"/>
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
-      <c r="Y20" s="23"/>
+      <c r="Y20" s="21"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -3618,7 +3622,7 @@
       <c r="V21" s="18"/>
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
-      <c r="Y21" s="23"/>
+      <c r="Y21" s="21"/>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
@@ -3628,10 +3632,10 @@
       <c r="I22" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="21" t="s">
+      <c r="J22" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="K22" s="21"/>
+      <c r="K22" s="20"/>
       <c r="L22" s="18"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
@@ -3645,18 +3649,18 @@
       <c r="V22" s="18"/>
       <c r="W22" s="18"/>
       <c r="X22" s="18"/>
-      <c r="Y22" s="23"/>
+      <c r="Y22" s="21"/>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C23" s="6" t="s">
         <v>21</v>
       </c>
       <c r="H23" s="18"/>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
       <c r="L23" s="18"/>
       <c r="M23" s="18"/>
       <c r="N23" s="18"/>
@@ -3670,7 +3674,7 @@
       <c r="V23" s="18"/>
       <c r="W23" s="18"/>
       <c r="X23" s="18"/>
-      <c r="Y23" s="23"/>
+      <c r="Y23" s="21"/>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
@@ -3679,11 +3683,11 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="H24" s="18"/>
-      <c r="I24" s="16" t="s">
+      <c r="I24" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
       <c r="L24" s="18"/>
       <c r="M24" s="18"/>
       <c r="N24" s="18"/>
@@ -3697,18 +3701,18 @@
       <c r="V24" s="18"/>
       <c r="W24" s="18"/>
       <c r="X24" s="18"/>
-      <c r="Y24" s="23"/>
+      <c r="Y24" s="21"/>
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>22</v>
       </c>
       <c r="H25" s="18"/>
-      <c r="I25" s="21" t="s">
+      <c r="I25" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
       <c r="L25" s="18"/>
       <c r="M25" s="18"/>
       <c r="N25" s="18"/>
@@ -3722,7 +3726,7 @@
       <c r="V25" s="18"/>
       <c r="W25" s="18"/>
       <c r="X25" s="18"/>
-      <c r="Y25" s="23"/>
+      <c r="Y25" s="21"/>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -3747,18 +3751,18 @@
       <c r="V26" s="18"/>
       <c r="W26" s="18"/>
       <c r="X26" s="18"/>
-      <c r="Y26" s="23"/>
+      <c r="Y26" s="21"/>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>14</v>
       </c>
       <c r="H27" s="18"/>
-      <c r="I27" s="21" t="s">
+      <c r="I27" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
       <c r="L27" s="18"/>
       <c r="M27" s="18"/>
       <c r="N27" s="18"/>
@@ -3772,18 +3776,18 @@
       <c r="V27" s="18"/>
       <c r="W27" s="18"/>
       <c r="X27" s="18"/>
-      <c r="Y27" s="23"/>
+      <c r="Y27" s="21"/>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>11</v>
       </c>
       <c r="H28" s="18"/>
-      <c r="I28" s="21" t="s">
+      <c r="I28" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
       <c r="L28" s="18"/>
       <c r="M28" s="18"/>
       <c r="N28" s="18"/>
@@ -3797,7 +3801,7 @@
       <c r="V28" s="18"/>
       <c r="W28" s="18"/>
       <c r="X28" s="18"/>
-      <c r="Y28" s="23"/>
+      <c r="Y28" s="21"/>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -3822,7 +3826,7 @@
       <c r="V29" s="18"/>
       <c r="W29" s="18"/>
       <c r="X29" s="18"/>
-      <c r="Y29" s="23"/>
+      <c r="Y29" s="21"/>
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
@@ -3832,10 +3836,10 @@
       <c r="I30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J30" s="17" t="s">
+      <c r="J30" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="K30" s="17"/>
+      <c r="K30" s="25"/>
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
       <c r="N30" s="18"/>
@@ -3849,18 +3853,18 @@
       <c r="V30" s="18"/>
       <c r="W30" s="18"/>
       <c r="X30" s="18"/>
-      <c r="Y30" s="23"/>
+      <c r="Y30" s="21"/>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>21</v>
       </c>
       <c r="H31" s="18"/>
-      <c r="I31" s="21" t="s">
+      <c r="I31" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
       <c r="N31" s="18"/>
@@ -3874,7 +3878,7 @@
       <c r="V31" s="18"/>
       <c r="W31" s="18"/>
       <c r="X31" s="18"/>
-      <c r="Y31" s="23"/>
+      <c r="Y31" s="21"/>
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
@@ -3899,7 +3903,7 @@
       <c r="V32" s="18"/>
       <c r="W32" s="18"/>
       <c r="X32" s="18"/>
-      <c r="Y32" s="23"/>
+      <c r="Y32" s="21"/>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
@@ -3907,11 +3911,11 @@
       </c>
       <c r="C33" s="6"/>
       <c r="H33" s="18"/>
-      <c r="I33" s="17" t="s">
+      <c r="I33" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
       <c r="N33" s="18"/>
@@ -3925,7 +3929,7 @@
       <c r="V33" s="18"/>
       <c r="W33" s="18"/>
       <c r="X33" s="18"/>
-      <c r="Y33" s="23"/>
+      <c r="Y33" s="21"/>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
@@ -3933,11 +3937,11 @@
       </c>
       <c r="C34" s="6"/>
       <c r="H34" s="18"/>
-      <c r="I34" s="19" t="s">
+      <c r="I34" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
       <c r="L34" s="18"/>
       <c r="M34" s="18"/>
       <c r="N34" s="18"/>
@@ -3951,7 +3955,7 @@
       <c r="V34" s="18"/>
       <c r="W34" s="18"/>
       <c r="X34" s="18"/>
-      <c r="Y34" s="23"/>
+      <c r="Y34" s="21"/>
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
@@ -3961,11 +3965,11 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="H35" s="18"/>
-      <c r="I35" s="20" t="s">
+      <c r="I35" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
       <c r="L35" s="18"/>
       <c r="M35" s="18"/>
       <c r="N35" s="18"/>
@@ -3979,7 +3983,7 @@
       <c r="V35" s="18"/>
       <c r="W35" s="18"/>
       <c r="X35" s="18"/>
-      <c r="Y35" s="23"/>
+      <c r="Y35" s="21"/>
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
@@ -3989,11 +3993,11 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="H36" s="18"/>
-      <c r="I36" s="20" t="s">
+      <c r="I36" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
       <c r="L36" s="18"/>
       <c r="M36" s="18"/>
       <c r="N36" s="18"/>
@@ -4007,7 +4011,7 @@
       <c r="V36" s="18"/>
       <c r="W36" s="18"/>
       <c r="X36" s="18"/>
-      <c r="Y36" s="23"/>
+      <c r="Y36" s="21"/>
     </row>
     <row r="37" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
@@ -4017,11 +4021,11 @@
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="H37" s="18"/>
-      <c r="I37" s="16" t="s">
+      <c r="I37" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
       <c r="L37" s="18"/>
       <c r="M37" s="18"/>
       <c r="N37" s="18"/>
@@ -4035,7 +4039,7 @@
       <c r="V37" s="18"/>
       <c r="W37" s="18"/>
       <c r="X37" s="18"/>
-      <c r="Y37" s="23"/>
+      <c r="Y37" s="21"/>
     </row>
     <row r="38" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
@@ -4045,11 +4049,11 @@
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="H38" s="18"/>
-      <c r="I38" s="20" t="s">
+      <c r="I38" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
       <c r="L38" s="18"/>
       <c r="M38" s="18"/>
       <c r="N38" s="18"/>
@@ -4063,7 +4067,7 @@
       <c r="V38" s="18"/>
       <c r="W38" s="18"/>
       <c r="X38" s="18"/>
-      <c r="Y38" s="23"/>
+      <c r="Y38" s="21"/>
     </row>
     <row r="39" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
@@ -4073,11 +4077,11 @@
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="H39" s="18"/>
-      <c r="I39" s="20" t="s">
+      <c r="I39" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
       <c r="L39" s="18"/>
       <c r="M39" s="18"/>
       <c r="N39" s="18"/>
@@ -4091,7 +4095,7 @@
       <c r="V39" s="18"/>
       <c r="W39" s="18"/>
       <c r="X39" s="18"/>
-      <c r="Y39" s="23"/>
+      <c r="Y39" s="21"/>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
@@ -4101,11 +4105,11 @@
       </c>
       <c r="E40" s="6"/>
       <c r="H40" s="18"/>
-      <c r="I40" s="20" t="s">
+      <c r="I40" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
       <c r="L40" s="18"/>
       <c r="M40" s="18"/>
       <c r="N40" s="18"/>
@@ -4119,7 +4123,7 @@
       <c r="V40" s="18"/>
       <c r="W40" s="18"/>
       <c r="X40" s="18"/>
-      <c r="Y40" s="23"/>
+      <c r="Y40" s="21"/>
     </row>
     <row r="41" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
@@ -4129,11 +4133,11 @@
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="H41" s="18"/>
-      <c r="I41" s="16" t="s">
+      <c r="I41" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="J41" s="16"/>
-      <c r="K41" s="16"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
       <c r="L41" s="18"/>
       <c r="M41" s="18"/>
       <c r="N41" s="18"/>
@@ -4147,7 +4151,7 @@
       <c r="V41" s="18"/>
       <c r="W41" s="18"/>
       <c r="X41" s="18"/>
-      <c r="Y41" s="23"/>
+      <c r="Y41" s="21"/>
     </row>
     <row r="42" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
@@ -4157,11 +4161,11 @@
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="H42" s="18"/>
-      <c r="I42" s="20" t="s">
+      <c r="I42" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
       <c r="L42" s="18"/>
       <c r="M42" s="18"/>
       <c r="N42" s="18"/>
@@ -4175,7 +4179,7 @@
       <c r="V42" s="18"/>
       <c r="W42" s="18"/>
       <c r="X42" s="18"/>
-      <c r="Y42" s="23"/>
+      <c r="Y42" s="21"/>
     </row>
     <row r="43" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
@@ -4185,11 +4189,11 @@
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="H43" s="18"/>
-      <c r="I43" s="20" t="s">
+      <c r="I43" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
       <c r="L43" s="18"/>
       <c r="M43" s="18"/>
       <c r="N43" s="18"/>
@@ -4203,7 +4207,7 @@
       <c r="V43" s="18"/>
       <c r="W43" s="18"/>
       <c r="X43" s="18"/>
-      <c r="Y43" s="23"/>
+      <c r="Y43" s="21"/>
     </row>
     <row r="44" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
@@ -4213,11 +4217,11 @@
       </c>
       <c r="E44" s="6"/>
       <c r="H44" s="18"/>
-      <c r="I44" s="20" t="s">
+      <c r="I44" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
+      <c r="J44" s="23"/>
+      <c r="K44" s="23"/>
       <c r="L44" s="18"/>
       <c r="M44" s="18"/>
       <c r="N44" s="18"/>
@@ -4231,7 +4235,7 @@
       <c r="V44" s="18"/>
       <c r="W44" s="18"/>
       <c r="X44" s="18"/>
-      <c r="Y44" s="23"/>
+      <c r="Y44" s="21"/>
     </row>
     <row r="45" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
@@ -4241,11 +4245,11 @@
         <v>11</v>
       </c>
       <c r="H45" s="18"/>
-      <c r="I45" s="20" t="s">
+      <c r="I45" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="23"/>
       <c r="L45" s="18"/>
       <c r="M45" s="18"/>
       <c r="N45" s="18"/>
@@ -4259,7 +4263,7 @@
       <c r="V45" s="18"/>
       <c r="W45" s="18"/>
       <c r="X45" s="18"/>
-      <c r="Y45" s="23"/>
+      <c r="Y45" s="21"/>
     </row>
     <row r="46" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
@@ -4269,11 +4273,11 @@
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="H46" s="18"/>
-      <c r="I46" s="16" t="s">
+      <c r="I46" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="J46" s="16"/>
-      <c r="K46" s="16"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
       <c r="L46" s="18"/>
       <c r="M46" s="18"/>
       <c r="N46" s="18"/>
@@ -4287,10 +4291,38 @@
       <c r="V46" s="18"/>
       <c r="W46" s="18"/>
       <c r="X46" s="18"/>
-      <c r="Y46" s="23"/>
+      <c r="Y46" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="Y10:Y46"/>
+    <mergeCell ref="L10:X46"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
     <mergeCell ref="H10:H46"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="I9:K9"/>
@@ -4307,34 +4339,6 @@
     <mergeCell ref="I21:K21"/>
     <mergeCell ref="I16:K16"/>
     <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="Y10:Y46"/>
-    <mergeCell ref="L10:X46"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="I45:K45"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="I31:K31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4376,28 +4380,28 @@
       <c r="H2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
       <c r="L2" s="9" t="s">
         <v>61</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21" t="s">
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
       <c r="U2" s="9" t="s">
         <v>65</v>
       </c>
@@ -4487,11 +4491,11 @@
       <c r="H9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
       <c r="L9" s="9" t="s">
         <v>95</v>
       </c>
@@ -4542,11 +4546,11 @@
       <c r="H10" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
       <c r="L10" s="18" t="s">
         <v>78</v>
       </c>
@@ -4562,7 +4566,7 @@
       <c r="V10" s="18"/>
       <c r="W10" s="18"/>
       <c r="X10" s="18"/>
-      <c r="Y10" s="23" t="s">
+      <c r="Y10" s="21" t="s">
         <v>127</v>
       </c>
     </row>
@@ -4571,11 +4575,11 @@
         <v>109</v>
       </c>
       <c r="H11" s="18"/>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
       <c r="L11" s="18"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
@@ -4589,18 +4593,18 @@
       <c r="V11" s="18"/>
       <c r="W11" s="18"/>
       <c r="X11" s="18"/>
-      <c r="Y11" s="23"/>
+      <c r="Y11" s="21"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>116</v>
       </c>
       <c r="H12" s="18"/>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
       <c r="L12" s="18"/>
       <c r="M12" s="18"/>
       <c r="N12" s="18"/>
@@ -4614,18 +4618,18 @@
       <c r="V12" s="18"/>
       <c r="W12" s="18"/>
       <c r="X12" s="18"/>
-      <c r="Y12" s="23"/>
+      <c r="Y12" s="21"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>117</v>
       </c>
       <c r="H13" s="18"/>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
       <c r="L13" s="18"/>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
@@ -4639,7 +4643,7 @@
       <c r="V13" s="18"/>
       <c r="W13" s="18"/>
       <c r="X13" s="18"/>
-      <c r="Y13" s="23"/>
+      <c r="Y13" s="21"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -4649,11 +4653,11 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="H14" s="18"/>
-      <c r="I14" s="20" t="s">
+      <c r="I14" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
       <c r="L14" s="18"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
@@ -4667,7 +4671,7 @@
       <c r="V14" s="18"/>
       <c r="W14" s="18"/>
       <c r="X14" s="18"/>
-      <c r="Y14" s="23"/>
+      <c r="Y14" s="21"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
@@ -4692,7 +4696,7 @@
       <c r="V15" s="18"/>
       <c r="W15" s="18"/>
       <c r="X15" s="18"/>
-      <c r="Y15" s="23"/>
+      <c r="Y15" s="21"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
@@ -4717,7 +4721,7 @@
       <c r="V16" s="18"/>
       <c r="W16" s="18"/>
       <c r="X16" s="18"/>
-      <c r="Y16" s="23"/>
+      <c r="Y16" s="21"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
@@ -4742,17 +4746,17 @@
       <c r="V17" s="18"/>
       <c r="W17" s="18"/>
       <c r="X17" s="18"/>
-      <c r="Y17" s="23"/>
+      <c r="Y17" s="21"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="H18" s="18"/>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="J18" s="16"/>
+      <c r="J18" s="19"/>
       <c r="K18" s="2" t="s">
         <v>135</v>
       </c>
@@ -4769,17 +4773,17 @@
       <c r="V18" s="18"/>
       <c r="W18" s="18"/>
       <c r="X18" s="18"/>
-      <c r="Y18" s="23"/>
+      <c r="Y18" s="21"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="H19" s="18"/>
-      <c r="I19" s="21" t="s">
+      <c r="I19" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="J19" s="21"/>
+      <c r="J19" s="20"/>
       <c r="K19" s="9" t="s">
         <v>95</v>
       </c>
@@ -4796,7 +4800,7 @@
       <c r="V19" s="18"/>
       <c r="W19" s="18"/>
       <c r="X19" s="18"/>
-      <c r="Y19" s="23"/>
+      <c r="Y19" s="21"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
@@ -4806,10 +4810,10 @@
       <c r="I20" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="J20" s="21" t="s">
+      <c r="J20" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="K20" s="21"/>
+      <c r="K20" s="20"/>
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
@@ -4823,7 +4827,7 @@
       <c r="V20" s="18"/>
       <c r="W20" s="18"/>
       <c r="X20" s="18"/>
-      <c r="Y20" s="23"/>
+      <c r="Y20" s="21"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -4833,10 +4837,10 @@
       <c r="I21" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="J21" s="17" t="s">
+      <c r="J21" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="K21" s="17"/>
+      <c r="K21" s="25"/>
       <c r="L21" s="18"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
@@ -4850,10 +4854,17 @@
       <c r="V21" s="18"/>
       <c r="W21" s="18"/>
       <c r="X21" s="18"/>
-      <c r="Y21" s="23"/>
+      <c r="Y21" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="Y10:Y21"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I19:J19"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
@@ -4866,13 +4877,6 @@
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="I13:K13"/>
     <mergeCell ref="J21:K21"/>
-    <mergeCell ref="Y10:Y21"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
New titles in utf8.xlsx
</commit_message>
<xml_diff>
--- a/doc/utf8.xlsx
+++ b/doc/utf8.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="16515" windowHeight="7995"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="16515" windowHeight="7995" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Errors" sheetId="7" r:id="rId1"/>
-    <sheet name="Automaton" sheetId="1" r:id="rId2"/>
-    <sheet name="Simplification I" sheetId="3" r:id="rId3"/>
-    <sheet name="Simplification II" sheetId="5" r:id="rId4"/>
-    <sheet name="Basic instructions" sheetId="2" r:id="rId5"/>
+    <sheet name="UTF-8 Errors" sheetId="7" r:id="rId1"/>
+    <sheet name="UTF-8 Automaton" sheetId="1" r:id="rId2"/>
+    <sheet name="UTF-8 Simplification I" sheetId="3" r:id="rId3"/>
+    <sheet name="UTF-8 Simplification II" sheetId="5" r:id="rId4"/>
+    <sheet name="UTF-8 Basic instructions" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -1158,28 +1158,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1484,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z46"/>
   <sheetViews>
-    <sheetView topLeftCell="D16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,28 +1682,28 @@
       <c r="I2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
       <c r="M2" s="8" t="s">
         <v>61</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O2" s="20" t="s">
+      <c r="O2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20" t="s">
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
       <c r="V2" s="8" t="s">
         <v>65</v>
       </c>
@@ -1793,11 +1793,11 @@
       <c r="I9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
       <c r="M9" s="8" t="s">
         <v>121</v>
       </c>
@@ -1845,30 +1845,30 @@
       <c r="B10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="18" t="s">
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="21" t="s">
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="21"/>
+      <c r="Z10" s="25" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1876,81 +1876,81 @@
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="22" t="s">
+      <c r="I11" s="21"/>
+      <c r="J11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="21"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="21"/>
+      <c r="Z11" s="25"/>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="19" t="s">
+      <c r="I12" s="21"/>
+      <c r="J12" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="19"/>
+      <c r="K12" s="18"/>
       <c r="L12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="21"/>
+      <c r="Z12" s="25"/>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="18" t="s">
+      <c r="I13" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="18" t="s">
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="21"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="21"/>
       <c r="Z13" s="12" t="s">
         <v>129</v>
       </c>
@@ -1959,27 +1959,27 @@
       <c r="C14" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="22" t="s">
+      <c r="I14" s="21"/>
+      <c r="J14" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="18" t="s">
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="18"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="21"/>
+      <c r="W14" s="21"/>
+      <c r="X14" s="21"/>
+      <c r="Y14" s="21"/>
       <c r="Z14" s="12" t="s">
         <v>129</v>
       </c>
@@ -1991,26 +1991,26 @@
       <c r="I15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="J15" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="19" t="s">
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="19"/>
-      <c r="V15" s="19"/>
-      <c r="W15" s="19"/>
-      <c r="X15" s="19"/>
-      <c r="Y15" s="19"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
       <c r="Z15" s="14" t="s">
         <v>128</v>
       </c>
@@ -2022,26 +2022,26 @@
       <c r="I16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="J16" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="18" t="s">
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="18"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21"/>
+      <c r="V16" s="21"/>
+      <c r="W16" s="21"/>
+      <c r="X16" s="21"/>
+      <c r="Y16" s="21"/>
       <c r="Z16" s="12" t="s">
         <v>129</v>
       </c>
@@ -2053,28 +2053,28 @@
       <c r="I17" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="20"/>
+      <c r="K17" s="23"/>
       <c r="L17" t="s">
         <v>57</v>
       </c>
-      <c r="M17" s="19" t="s">
+      <c r="M17" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="19"/>
-      <c r="W17" s="19"/>
-      <c r="X17" s="19"/>
-      <c r="Y17" s="19"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
+      <c r="U17" s="18"/>
+      <c r="V17" s="18"/>
+      <c r="W17" s="18"/>
+      <c r="X17" s="18"/>
+      <c r="Y17" s="18"/>
       <c r="Z17" s="14" t="s">
         <v>128</v>
       </c>
@@ -2086,26 +2086,26 @@
       <c r="I18" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J18" s="22" t="s">
+      <c r="J18" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="18" t="s">
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="18"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="21"/>
       <c r="Z18" s="12" t="s">
         <v>129</v>
       </c>
@@ -2117,26 +2117,26 @@
       <c r="I19" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="J19" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="18" t="s">
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="18"/>
-      <c r="X19" s="18"/>
-      <c r="Y19" s="18"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="21"/>
+      <c r="W19" s="21"/>
+      <c r="X19" s="21"/>
+      <c r="Y19" s="21"/>
       <c r="Z19" s="12" t="s">
         <v>129</v>
       </c>
@@ -2148,26 +2148,26 @@
       <c r="I20" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="20" t="s">
+      <c r="J20" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="19" t="s">
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="19"/>
-      <c r="S20" s="19"/>
-      <c r="T20" s="19"/>
-      <c r="U20" s="19"/>
-      <c r="V20" s="19"/>
-      <c r="W20" s="19"/>
-      <c r="X20" s="19"/>
-      <c r="Y20" s="19"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="18"/>
+      <c r="U20" s="18"/>
+      <c r="V20" s="18"/>
+      <c r="W20" s="18"/>
+      <c r="X20" s="18"/>
+      <c r="Y20" s="18"/>
       <c r="Z20" s="14" t="s">
         <v>128</v>
       </c>
@@ -2179,26 +2179,26 @@
       <c r="I21" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="22" t="s">
+      <c r="J21" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="18" t="s">
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
-      <c r="T21" s="18"/>
-      <c r="U21" s="18"/>
-      <c r="V21" s="18"/>
-      <c r="W21" s="18"/>
-      <c r="X21" s="18"/>
-      <c r="Y21" s="18"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="21"/>
+      <c r="V21" s="21"/>
+      <c r="W21" s="21"/>
+      <c r="X21" s="21"/>
+      <c r="Y21" s="21"/>
       <c r="Z21" s="12" t="s">
         <v>129</v>
       </c>
@@ -2213,25 +2213,25 @@
       <c r="J22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K22" s="20" t="s">
+      <c r="K22" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="L22" s="20"/>
-      <c r="M22" s="19" t="s">
+      <c r="L22" s="23"/>
+      <c r="M22" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
-      <c r="R22" s="19"/>
-      <c r="S22" s="19"/>
-      <c r="T22" s="19"/>
-      <c r="U22" s="19"/>
-      <c r="V22" s="19"/>
-      <c r="W22" s="19"/>
-      <c r="X22" s="19"/>
-      <c r="Y22" s="19"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="18"/>
+      <c r="U22" s="18"/>
+      <c r="V22" s="18"/>
+      <c r="W22" s="18"/>
+      <c r="X22" s="18"/>
+      <c r="Y22" s="18"/>
       <c r="Z22" s="14" t="s">
         <v>128</v>
       </c>
@@ -2243,26 +2243,26 @@
       <c r="I23" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J23" s="23" t="s">
+      <c r="J23" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="18" t="s">
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
-      <c r="T23" s="18"/>
-      <c r="U23" s="18"/>
-      <c r="V23" s="18"/>
-      <c r="W23" s="18"/>
-      <c r="X23" s="18"/>
-      <c r="Y23" s="18"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="21"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="21"/>
+      <c r="V23" s="21"/>
+      <c r="W23" s="21"/>
+      <c r="X23" s="21"/>
+      <c r="Y23" s="21"/>
       <c r="Z23" s="12" t="s">
         <v>129</v>
       </c>
@@ -2275,26 +2275,26 @@
       <c r="I24" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J24" s="19" t="s">
+      <c r="J24" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19" t="s">
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="19"/>
-      <c r="S24" s="19"/>
-      <c r="T24" s="19"/>
-      <c r="U24" s="19"/>
-      <c r="V24" s="19"/>
-      <c r="W24" s="19"/>
-      <c r="X24" s="19"/>
-      <c r="Y24" s="19"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="18"/>
+      <c r="U24" s="18"/>
+      <c r="V24" s="18"/>
+      <c r="W24" s="18"/>
+      <c r="X24" s="18"/>
+      <c r="Y24" s="18"/>
       <c r="Z24" s="10" t="s">
         <v>132</v>
       </c>
@@ -2306,26 +2306,26 @@
       <c r="I25" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J25" s="20" t="s">
+      <c r="J25" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="18" t="s">
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="18"/>
-      <c r="T25" s="18"/>
-      <c r="U25" s="18"/>
-      <c r="V25" s="18"/>
-      <c r="W25" s="18"/>
-      <c r="X25" s="18"/>
-      <c r="Y25" s="18"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="21"/>
+      <c r="W25" s="21"/>
+      <c r="X25" s="21"/>
+      <c r="Y25" s="21"/>
       <c r="Z25" s="12" t="s">
         <v>129</v>
       </c>
@@ -2337,26 +2337,26 @@
       <c r="I26" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J26" s="22" t="s">
+      <c r="J26" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="19" t="s">
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="19"/>
-      <c r="S26" s="19"/>
-      <c r="T26" s="19"/>
-      <c r="U26" s="19"/>
-      <c r="V26" s="19"/>
-      <c r="W26" s="19"/>
-      <c r="X26" s="19"/>
-      <c r="Y26" s="19"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="18"/>
+      <c r="U26" s="18"/>
+      <c r="V26" s="18"/>
+      <c r="W26" s="18"/>
+      <c r="X26" s="18"/>
+      <c r="Y26" s="18"/>
       <c r="Z26" s="10" t="s">
         <v>132</v>
       </c>
@@ -2368,26 +2368,26 @@
       <c r="I27" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J27" s="20" t="s">
+      <c r="J27" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="19" t="s">
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="19"/>
-      <c r="S27" s="19"/>
-      <c r="T27" s="19"/>
-      <c r="U27" s="19"/>
-      <c r="V27" s="19"/>
-      <c r="W27" s="19"/>
-      <c r="X27" s="19"/>
-      <c r="Y27" s="19"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
+      <c r="T27" s="18"/>
+      <c r="U27" s="18"/>
+      <c r="V27" s="18"/>
+      <c r="W27" s="18"/>
+      <c r="X27" s="18"/>
+      <c r="Y27" s="18"/>
       <c r="Z27" s="14" t="s">
         <v>128</v>
       </c>
@@ -2399,26 +2399,26 @@
       <c r="I28" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J28" s="20" t="s">
+      <c r="J28" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="18" t="s">
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
-      <c r="T28" s="18"/>
-      <c r="U28" s="18"/>
-      <c r="V28" s="18"/>
-      <c r="W28" s="18"/>
-      <c r="X28" s="18"/>
-      <c r="Y28" s="18"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="21"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="21"/>
+      <c r="U28" s="21"/>
+      <c r="V28" s="21"/>
+      <c r="W28" s="21"/>
+      <c r="X28" s="21"/>
+      <c r="Y28" s="21"/>
       <c r="Z28" s="12" t="s">
         <v>129</v>
       </c>
@@ -2430,26 +2430,26 @@
       <c r="I29" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J29" s="22" t="s">
+      <c r="J29" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="19" t="s">
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="N29" s="19"/>
-      <c r="O29" s="19"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
-      <c r="S29" s="19"/>
-      <c r="T29" s="19"/>
-      <c r="U29" s="19"/>
-      <c r="V29" s="19"/>
-      <c r="W29" s="19"/>
-      <c r="X29" s="19"/>
-      <c r="Y29" s="19"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+      <c r="V29" s="18"/>
+      <c r="W29" s="18"/>
+      <c r="X29" s="18"/>
+      <c r="Y29" s="18"/>
       <c r="Z29" s="10" t="s">
         <v>132</v>
       </c>
@@ -2464,25 +2464,25 @@
       <c r="J30" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K30" s="25" t="s">
+      <c r="K30" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="L30" s="25"/>
-      <c r="M30" s="19" t="s">
+      <c r="L30" s="20"/>
+      <c r="M30" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="19"/>
-      <c r="S30" s="19"/>
-      <c r="T30" s="19"/>
-      <c r="U30" s="19"/>
-      <c r="V30" s="19"/>
-      <c r="W30" s="19"/>
-      <c r="X30" s="19"/>
-      <c r="Y30" s="19"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="18"/>
+      <c r="U30" s="18"/>
+      <c r="V30" s="18"/>
+      <c r="W30" s="18"/>
+      <c r="X30" s="18"/>
+      <c r="Y30" s="18"/>
       <c r="Z30" s="14" t="s">
         <v>128</v>
       </c>
@@ -2494,26 +2494,26 @@
       <c r="I31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J31" s="20" t="s">
+      <c r="J31" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="18" t="s">
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
-      <c r="T31" s="18"/>
-      <c r="U31" s="18"/>
-      <c r="V31" s="18"/>
-      <c r="W31" s="18"/>
-      <c r="X31" s="18"/>
-      <c r="Y31" s="18"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="21"/>
+      <c r="W31" s="21"/>
+      <c r="X31" s="21"/>
+      <c r="Y31" s="21"/>
       <c r="Z31" s="12" t="s">
         <v>129</v>
       </c>
@@ -2525,26 +2525,26 @@
       <c r="I32" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J32" s="22" t="s">
+      <c r="J32" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="19" t="s">
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="19"/>
-      <c r="W32" s="19"/>
-      <c r="X32" s="19"/>
-      <c r="Y32" s="19"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="18"/>
+      <c r="U32" s="18"/>
+      <c r="V32" s="18"/>
+      <c r="W32" s="18"/>
+      <c r="X32" s="18"/>
+      <c r="Y32" s="18"/>
       <c r="Z32" s="10" t="s">
         <v>132</v>
       </c>
@@ -2556,26 +2556,26 @@
       <c r="I33" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="J33" s="25" t="s">
+      <c r="J33" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="18" t="s">
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
-      <c r="T33" s="18"/>
-      <c r="U33" s="18"/>
-      <c r="V33" s="18"/>
-      <c r="W33" s="18"/>
-      <c r="X33" s="18"/>
-      <c r="Y33" s="18"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="21"/>
+      <c r="Q33" s="21"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="21"/>
+      <c r="U33" s="21"/>
+      <c r="V33" s="21"/>
+      <c r="W33" s="21"/>
+      <c r="X33" s="21"/>
+      <c r="Y33" s="21"/>
       <c r="Z33" s="12" t="s">
         <v>129</v>
       </c>
@@ -2588,26 +2588,26 @@
       <c r="I34" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="J34" s="24" t="s">
+      <c r="J34" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="19" t="s">
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
-      <c r="S34" s="19"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
-      <c r="V34" s="19"/>
-      <c r="W34" s="19"/>
-      <c r="X34" s="19"/>
-      <c r="Y34" s="19"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="18"/>
+      <c r="U34" s="18"/>
+      <c r="V34" s="18"/>
+      <c r="W34" s="18"/>
+      <c r="X34" s="18"/>
+      <c r="Y34" s="18"/>
       <c r="Z34" s="10" t="s">
         <v>132</v>
       </c>
@@ -2623,26 +2623,26 @@
       <c r="I35" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J35" s="23" t="s">
+      <c r="J35" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="K35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="19" t="s">
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="19"/>
-      <c r="R35" s="19"/>
-      <c r="S35" s="19"/>
-      <c r="T35" s="19"/>
-      <c r="U35" s="19"/>
-      <c r="V35" s="19"/>
-      <c r="W35" s="19"/>
-      <c r="X35" s="19"/>
-      <c r="Y35" s="19"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="18"/>
+      <c r="U35" s="18"/>
+      <c r="V35" s="18"/>
+      <c r="W35" s="18"/>
+      <c r="X35" s="18"/>
+      <c r="Y35" s="18"/>
       <c r="Z35" s="14" t="s">
         <v>128</v>
       </c>
@@ -2658,26 +2658,26 @@
       <c r="I36" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J36" s="23" t="s">
+      <c r="J36" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="K36" s="23"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="18" t="s">
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="18"/>
-      <c r="T36" s="18"/>
-      <c r="U36" s="18"/>
-      <c r="V36" s="18"/>
-      <c r="W36" s="18"/>
-      <c r="X36" s="18"/>
-      <c r="Y36" s="18"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
+      <c r="Q36" s="21"/>
+      <c r="R36" s="21"/>
+      <c r="S36" s="21"/>
+      <c r="T36" s="21"/>
+      <c r="U36" s="21"/>
+      <c r="V36" s="21"/>
+      <c r="W36" s="21"/>
+      <c r="X36" s="21"/>
+      <c r="Y36" s="21"/>
       <c r="Z36" s="12" t="s">
         <v>129</v>
       </c>
@@ -2693,26 +2693,26 @@
       <c r="I37" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J37" s="19" t="s">
+      <c r="J37" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19" t="s">
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="19"/>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
-      <c r="U37" s="19"/>
-      <c r="V37" s="19"/>
-      <c r="W37" s="19"/>
-      <c r="X37" s="19"/>
-      <c r="Y37" s="19"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="18"/>
+      <c r="S37" s="18"/>
+      <c r="T37" s="18"/>
+      <c r="U37" s="18"/>
+      <c r="V37" s="18"/>
+      <c r="W37" s="18"/>
+      <c r="X37" s="18"/>
+      <c r="Y37" s="18"/>
       <c r="Z37" s="10" t="s">
         <v>132</v>
       </c>
@@ -2728,26 +2728,26 @@
       <c r="I38" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J38" s="23" t="s">
+      <c r="J38" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="K38" s="23"/>
-      <c r="L38" s="23"/>
-      <c r="M38" s="19" t="s">
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
-      <c r="R38" s="19"/>
-      <c r="S38" s="19"/>
-      <c r="T38" s="19"/>
-      <c r="U38" s="19"/>
-      <c r="V38" s="19"/>
-      <c r="W38" s="19"/>
-      <c r="X38" s="19"/>
-      <c r="Y38" s="19"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18"/>
+      <c r="S38" s="18"/>
+      <c r="T38" s="18"/>
+      <c r="U38" s="18"/>
+      <c r="V38" s="18"/>
+      <c r="W38" s="18"/>
+      <c r="X38" s="18"/>
+      <c r="Y38" s="18"/>
       <c r="Z38" s="14" t="s">
         <v>128</v>
       </c>
@@ -2763,26 +2763,26 @@
       <c r="I39" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J39" s="23" t="s">
+      <c r="J39" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="K39" s="23"/>
-      <c r="L39" s="23"/>
-      <c r="M39" s="18" t="s">
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="18"/>
-      <c r="U39" s="18"/>
-      <c r="V39" s="18"/>
-      <c r="W39" s="18"/>
-      <c r="X39" s="18"/>
-      <c r="Y39" s="18"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="21"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="21"/>
+      <c r="T39" s="21"/>
+      <c r="U39" s="21"/>
+      <c r="V39" s="21"/>
+      <c r="W39" s="21"/>
+      <c r="X39" s="21"/>
+      <c r="Y39" s="21"/>
       <c r="Z39" s="12" t="s">
         <v>129</v>
       </c>
@@ -2798,26 +2798,26 @@
       <c r="I40" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J40" s="23" t="s">
+      <c r="J40" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="K40" s="23"/>
-      <c r="L40" s="23"/>
-      <c r="M40" s="19" t="s">
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
-      <c r="P40" s="19"/>
-      <c r="Q40" s="19"/>
-      <c r="R40" s="19"/>
-      <c r="S40" s="19"/>
-      <c r="T40" s="19"/>
-      <c r="U40" s="19"/>
-      <c r="V40" s="19"/>
-      <c r="W40" s="19"/>
-      <c r="X40" s="19"/>
-      <c r="Y40" s="19"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
+      <c r="T40" s="18"/>
+      <c r="U40" s="18"/>
+      <c r="V40" s="18"/>
+      <c r="W40" s="18"/>
+      <c r="X40" s="18"/>
+      <c r="Y40" s="18"/>
       <c r="Z40" s="10" t="s">
         <v>132</v>
       </c>
@@ -2833,26 +2833,26 @@
       <c r="I41" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="J41" s="19" t="s">
+      <c r="J41" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19" t="s">
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="N41" s="19"/>
-      <c r="O41" s="19"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="19"/>
-      <c r="R41" s="19"/>
-      <c r="S41" s="19"/>
-      <c r="T41" s="19"/>
-      <c r="U41" s="19"/>
-      <c r="V41" s="19"/>
-      <c r="W41" s="19"/>
-      <c r="X41" s="19"/>
-      <c r="Y41" s="19"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
+      <c r="T41" s="18"/>
+      <c r="U41" s="18"/>
+      <c r="V41" s="18"/>
+      <c r="W41" s="18"/>
+      <c r="X41" s="18"/>
+      <c r="Y41" s="18"/>
       <c r="Z41" s="10" t="s">
         <v>131</v>
       </c>
@@ -2868,26 +2868,26 @@
       <c r="I42" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J42" s="23" t="s">
+      <c r="J42" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="K42" s="23"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="19" t="s">
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="N42" s="19"/>
-      <c r="O42" s="19"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="19"/>
-      <c r="R42" s="19"/>
-      <c r="S42" s="19"/>
-      <c r="T42" s="19"/>
-      <c r="U42" s="19"/>
-      <c r="V42" s="19"/>
-      <c r="W42" s="19"/>
-      <c r="X42" s="19"/>
-      <c r="Y42" s="19"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="18"/>
+      <c r="Q42" s="18"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="18"/>
+      <c r="T42" s="18"/>
+      <c r="U42" s="18"/>
+      <c r="V42" s="18"/>
+      <c r="W42" s="18"/>
+      <c r="X42" s="18"/>
+      <c r="Y42" s="18"/>
       <c r="Z42" s="14" t="s">
         <v>128</v>
       </c>
@@ -2903,26 +2903,26 @@
       <c r="I43" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J43" s="23" t="s">
+      <c r="J43" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="K43" s="23"/>
-      <c r="L43" s="23"/>
-      <c r="M43" s="18" t="s">
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
-      <c r="T43" s="18"/>
-      <c r="U43" s="18"/>
-      <c r="V43" s="18"/>
-      <c r="W43" s="18"/>
-      <c r="X43" s="18"/>
-      <c r="Y43" s="18"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
+      <c r="P43" s="21"/>
+      <c r="Q43" s="21"/>
+      <c r="R43" s="21"/>
+      <c r="S43" s="21"/>
+      <c r="T43" s="21"/>
+      <c r="U43" s="21"/>
+      <c r="V43" s="21"/>
+      <c r="W43" s="21"/>
+      <c r="X43" s="21"/>
+      <c r="Y43" s="21"/>
       <c r="Z43" s="12" t="s">
         <v>129</v>
       </c>
@@ -2938,26 +2938,26 @@
       <c r="I44" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="J44" s="23" t="s">
+      <c r="J44" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="K44" s="23"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="19" t="s">
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="N44" s="19"/>
-      <c r="O44" s="19"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="19"/>
-      <c r="R44" s="19"/>
-      <c r="S44" s="19"/>
-      <c r="T44" s="19"/>
-      <c r="U44" s="19"/>
-      <c r="V44" s="19"/>
-      <c r="W44" s="19"/>
-      <c r="X44" s="19"/>
-      <c r="Y44" s="19"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
+      <c r="T44" s="18"/>
+      <c r="U44" s="18"/>
+      <c r="V44" s="18"/>
+      <c r="W44" s="18"/>
+      <c r="X44" s="18"/>
+      <c r="Y44" s="18"/>
       <c r="Z44" s="10" t="s">
         <v>132</v>
       </c>
@@ -2973,26 +2973,26 @@
       <c r="I45" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="J45" s="23" t="s">
+      <c r="J45" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="K45" s="23"/>
-      <c r="L45" s="23"/>
-      <c r="M45" s="19" t="s">
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="N45" s="19"/>
-      <c r="O45" s="19"/>
-      <c r="P45" s="19"/>
-      <c r="Q45" s="19"/>
-      <c r="R45" s="19"/>
-      <c r="S45" s="19"/>
-      <c r="T45" s="19"/>
-      <c r="U45" s="19"/>
-      <c r="V45" s="19"/>
-      <c r="W45" s="19"/>
-      <c r="X45" s="19"/>
-      <c r="Y45" s="19"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18"/>
+      <c r="S45" s="18"/>
+      <c r="T45" s="18"/>
+      <c r="U45" s="18"/>
+      <c r="V45" s="18"/>
+      <c r="W45" s="18"/>
+      <c r="X45" s="18"/>
+      <c r="Y45" s="18"/>
       <c r="Z45" s="10" t="s">
         <v>131</v>
       </c>
@@ -3008,77 +3008,50 @@
       <c r="I46" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="J46" s="19" t="s">
+      <c r="J46" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="K46" s="19"/>
-      <c r="L46" s="19"/>
-      <c r="M46" s="19" t="s">
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="N46" s="19"/>
-      <c r="O46" s="19"/>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="19"/>
-      <c r="R46" s="19"/>
-      <c r="S46" s="19"/>
-      <c r="T46" s="19"/>
-      <c r="U46" s="19"/>
-      <c r="V46" s="19"/>
-      <c r="W46" s="19"/>
-      <c r="X46" s="19"/>
-      <c r="Y46" s="19"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18"/>
+      <c r="S46" s="18"/>
+      <c r="T46" s="18"/>
+      <c r="U46" s="18"/>
+      <c r="V46" s="18"/>
+      <c r="W46" s="18"/>
+      <c r="X46" s="18"/>
+      <c r="Y46" s="18"/>
       <c r="Z46" s="10" t="s">
         <v>130</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="J45:L45"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M33:Y33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="M34:Y34"/>
-    <mergeCell ref="M36:Y36"/>
-    <mergeCell ref="M27:Y27"/>
-    <mergeCell ref="M30:Y30"/>
-    <mergeCell ref="M35:Y35"/>
-    <mergeCell ref="M46:Y46"/>
-    <mergeCell ref="M43:Y43"/>
-    <mergeCell ref="M40:Y40"/>
-    <mergeCell ref="M39:Y39"/>
-    <mergeCell ref="M23:Y23"/>
-    <mergeCell ref="M24:Y24"/>
-    <mergeCell ref="M26:Y26"/>
-    <mergeCell ref="M29:Y29"/>
-    <mergeCell ref="M32:Y32"/>
-    <mergeCell ref="M25:Y25"/>
-    <mergeCell ref="M28:Y28"/>
-    <mergeCell ref="M31:Y31"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="M38:Y38"/>
-    <mergeCell ref="M42:Y42"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="M37:Y37"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="M44:Y44"/>
-    <mergeCell ref="M41:Y41"/>
-    <mergeCell ref="M45:Y45"/>
+    <mergeCell ref="Z10:Z12"/>
+    <mergeCell ref="M17:Y17"/>
+    <mergeCell ref="M20:Y20"/>
+    <mergeCell ref="M22:Y22"/>
+    <mergeCell ref="M16:Y16"/>
+    <mergeCell ref="M18:Y18"/>
+    <mergeCell ref="M19:Y19"/>
+    <mergeCell ref="M21:Y21"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M13:Y13"/>
+    <mergeCell ref="M14:Y14"/>
+    <mergeCell ref="M10:Y12"/>
+    <mergeCell ref="M15:Y15"/>
+    <mergeCell ref="J12:K12"/>
     <mergeCell ref="I10:I12"/>
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="J32:L32"/>
@@ -3091,28 +3064,55 @@
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M13:Y13"/>
-    <mergeCell ref="M14:Y14"/>
-    <mergeCell ref="M10:Y12"/>
-    <mergeCell ref="M15:Y15"/>
     <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J12:K12"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="K22:L22"/>
-    <mergeCell ref="Z10:Z12"/>
-    <mergeCell ref="M17:Y17"/>
-    <mergeCell ref="M20:Y20"/>
-    <mergeCell ref="M22:Y22"/>
-    <mergeCell ref="M16:Y16"/>
     <mergeCell ref="J16:L16"/>
-    <mergeCell ref="M18:Y18"/>
-    <mergeCell ref="M19:Y19"/>
-    <mergeCell ref="M21:Y21"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="M37:Y37"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="M23:Y23"/>
+    <mergeCell ref="M24:Y24"/>
+    <mergeCell ref="M26:Y26"/>
+    <mergeCell ref="M29:Y29"/>
+    <mergeCell ref="M32:Y32"/>
+    <mergeCell ref="M25:Y25"/>
+    <mergeCell ref="M28:Y28"/>
+    <mergeCell ref="M31:Y31"/>
+    <mergeCell ref="M36:Y36"/>
+    <mergeCell ref="M27:Y27"/>
+    <mergeCell ref="M30:Y30"/>
+    <mergeCell ref="M35:Y35"/>
+    <mergeCell ref="M46:Y46"/>
+    <mergeCell ref="M43:Y43"/>
+    <mergeCell ref="M40:Y40"/>
+    <mergeCell ref="M39:Y39"/>
+    <mergeCell ref="M38:Y38"/>
+    <mergeCell ref="M42:Y42"/>
+    <mergeCell ref="M44:Y44"/>
+    <mergeCell ref="M41:Y41"/>
+    <mergeCell ref="M45:Y45"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M33:Y33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="M34:Y34"/>
+    <mergeCell ref="J46:L46"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="J45:L45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3153,28 +3153,28 @@
       <c r="H2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
       <c r="L2" s="9" t="s">
         <v>61</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20" t="s">
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
       <c r="U2" s="9" t="s">
         <v>65</v>
       </c>
@@ -3264,11 +3264,11 @@
       <c r="H9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
       <c r="L9" s="9" t="s">
         <v>4</v>
       </c>
@@ -3316,30 +3316,30 @@
       <c r="B10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="18" t="s">
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="21" t="s">
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="25" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3347,334 +3347,334 @@
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="22" t="s">
+      <c r="H11" s="21"/>
+      <c r="I11" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="21"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="25"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="23" t="s">
+      <c r="H12" s="21"/>
+      <c r="I12" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="J12" s="19"/>
+      <c r="J12" s="18"/>
       <c r="K12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="25"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>92</v>
       </c>
       <c r="C13" s="6"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="19" t="s">
+      <c r="H13" s="21"/>
+      <c r="I13" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="21"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="21"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="25"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>80</v>
       </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="22" t="s">
+      <c r="H14" s="21"/>
+      <c r="I14" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="21"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="21"/>
+      <c r="W14" s="21"/>
+      <c r="X14" s="21"/>
+      <c r="Y14" s="25"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="18"/>
-      <c r="I15" s="20" t="s">
+      <c r="H15" s="21"/>
+      <c r="I15" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="21"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="21"/>
+      <c r="W15" s="21"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="25"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>81</v>
       </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="22" t="s">
+      <c r="H16" s="21"/>
+      <c r="I16" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="21"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21"/>
+      <c r="V16" s="21"/>
+      <c r="W16" s="21"/>
+      <c r="X16" s="21"/>
+      <c r="Y16" s="25"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="18"/>
-      <c r="I17" s="20" t="s">
+      <c r="H17" s="21"/>
+      <c r="I17" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="J17" s="20"/>
+      <c r="J17" s="23"/>
       <c r="K17" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
-      <c r="X17" s="18"/>
-      <c r="Y17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="21"/>
+      <c r="V17" s="21"/>
+      <c r="W17" s="21"/>
+      <c r="X17" s="21"/>
+      <c r="Y17" s="25"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>82</v>
       </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="22" t="s">
+      <c r="H18" s="21"/>
+      <c r="I18" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="21"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="25"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="24" t="s">
+      <c r="H19" s="21"/>
+      <c r="I19" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="18"/>
-      <c r="X19" s="18"/>
-      <c r="Y19" s="21"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="21"/>
+      <c r="W19" s="21"/>
+      <c r="X19" s="21"/>
+      <c r="Y19" s="25"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="20" t="s">
+      <c r="H20" s="21"/>
+      <c r="I20" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
-      <c r="T20" s="18"/>
-      <c r="U20" s="18"/>
-      <c r="V20" s="18"/>
-      <c r="W20" s="18"/>
-      <c r="X20" s="18"/>
-      <c r="Y20" s="21"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="21"/>
+      <c r="W20" s="21"/>
+      <c r="X20" s="21"/>
+      <c r="Y20" s="25"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>83</v>
       </c>
-      <c r="H21" s="18"/>
-      <c r="I21" s="22" t="s">
+      <c r="H21" s="21"/>
+      <c r="I21" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
-      <c r="T21" s="18"/>
-      <c r="U21" s="18"/>
-      <c r="V21" s="18"/>
-      <c r="W21" s="18"/>
-      <c r="X21" s="18"/>
-      <c r="Y21" s="21"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="21"/>
+      <c r="V21" s="21"/>
+      <c r="W21" s="21"/>
+      <c r="X21" s="21"/>
+      <c r="Y21" s="25"/>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="18"/>
+      <c r="H22" s="21"/>
       <c r="I22" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="K22" s="20"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18"/>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18"/>
-      <c r="W22" s="18"/>
-      <c r="X22" s="18"/>
-      <c r="Y22" s="21"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="21"/>
+      <c r="W22" s="21"/>
+      <c r="X22" s="21"/>
+      <c r="Y22" s="25"/>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H23" s="18"/>
-      <c r="I23" s="23" t="s">
+      <c r="H23" s="21"/>
+      <c r="I23" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
-      <c r="T23" s="18"/>
-      <c r="U23" s="18"/>
-      <c r="V23" s="18"/>
-      <c r="W23" s="18"/>
-      <c r="X23" s="18"/>
-      <c r="Y23" s="21"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="21"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="21"/>
+      <c r="V23" s="21"/>
+      <c r="W23" s="21"/>
+      <c r="X23" s="21"/>
+      <c r="Y23" s="25"/>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
@@ -3682,280 +3682,280 @@
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="19" t="s">
+      <c r="H24" s="21"/>
+      <c r="I24" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
-      <c r="T24" s="18"/>
-      <c r="U24" s="18"/>
-      <c r="V24" s="18"/>
-      <c r="W24" s="18"/>
-      <c r="X24" s="18"/>
-      <c r="Y24" s="21"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21"/>
+      <c r="V24" s="21"/>
+      <c r="W24" s="21"/>
+      <c r="X24" s="21"/>
+      <c r="Y24" s="25"/>
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>22</v>
       </c>
-      <c r="H25" s="18"/>
-      <c r="I25" s="20" t="s">
+      <c r="H25" s="21"/>
+      <c r="I25" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="18"/>
-      <c r="T25" s="18"/>
-      <c r="U25" s="18"/>
-      <c r="V25" s="18"/>
-      <c r="W25" s="18"/>
-      <c r="X25" s="18"/>
-      <c r="Y25" s="21"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="21"/>
+      <c r="W25" s="21"/>
+      <c r="X25" s="21"/>
+      <c r="Y25" s="25"/>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>84</v>
       </c>
-      <c r="H26" s="18"/>
-      <c r="I26" s="22" t="s">
+      <c r="H26" s="21"/>
+      <c r="I26" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
-      <c r="T26" s="18"/>
-      <c r="U26" s="18"/>
-      <c r="V26" s="18"/>
-      <c r="W26" s="18"/>
-      <c r="X26" s="18"/>
-      <c r="Y26" s="21"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="21"/>
+      <c r="U26" s="21"/>
+      <c r="V26" s="21"/>
+      <c r="W26" s="21"/>
+      <c r="X26" s="21"/>
+      <c r="Y26" s="25"/>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="18"/>
-      <c r="I27" s="20" t="s">
+      <c r="H27" s="21"/>
+      <c r="I27" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
-      <c r="T27" s="18"/>
-      <c r="U27" s="18"/>
-      <c r="V27" s="18"/>
-      <c r="W27" s="18"/>
-      <c r="X27" s="18"/>
-      <c r="Y27" s="21"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="21"/>
+      <c r="T27" s="21"/>
+      <c r="U27" s="21"/>
+      <c r="V27" s="21"/>
+      <c r="W27" s="21"/>
+      <c r="X27" s="21"/>
+      <c r="Y27" s="25"/>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="18"/>
-      <c r="I28" s="20" t="s">
+      <c r="H28" s="21"/>
+      <c r="I28" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
-      <c r="T28" s="18"/>
-      <c r="U28" s="18"/>
-      <c r="V28" s="18"/>
-      <c r="W28" s="18"/>
-      <c r="X28" s="18"/>
-      <c r="Y28" s="21"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="21"/>
+      <c r="S28" s="21"/>
+      <c r="T28" s="21"/>
+      <c r="U28" s="21"/>
+      <c r="V28" s="21"/>
+      <c r="W28" s="21"/>
+      <c r="X28" s="21"/>
+      <c r="Y28" s="25"/>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>85</v>
       </c>
-      <c r="H29" s="18"/>
-      <c r="I29" s="22" t="s">
+      <c r="H29" s="21"/>
+      <c r="I29" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18"/>
-      <c r="S29" s="18"/>
-      <c r="T29" s="18"/>
-      <c r="U29" s="18"/>
-      <c r="V29" s="18"/>
-      <c r="W29" s="18"/>
-      <c r="X29" s="18"/>
-      <c r="Y29" s="21"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="21"/>
+      <c r="U29" s="21"/>
+      <c r="V29" s="21"/>
+      <c r="W29" s="21"/>
+      <c r="X29" s="21"/>
+      <c r="Y29" s="25"/>
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="18"/>
+      <c r="H30" s="21"/>
       <c r="I30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J30" s="25" t="s">
+      <c r="J30" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="K30" s="25"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
-      <c r="T30" s="18"/>
-      <c r="U30" s="18"/>
-      <c r="V30" s="18"/>
-      <c r="W30" s="18"/>
-      <c r="X30" s="18"/>
-      <c r="Y30" s="21"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21"/>
+      <c r="T30" s="21"/>
+      <c r="U30" s="21"/>
+      <c r="V30" s="21"/>
+      <c r="W30" s="21"/>
+      <c r="X30" s="21"/>
+      <c r="Y30" s="25"/>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>21</v>
       </c>
-      <c r="H31" s="18"/>
-      <c r="I31" s="20" t="s">
+      <c r="H31" s="21"/>
+      <c r="I31" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
-      <c r="T31" s="18"/>
-      <c r="U31" s="18"/>
-      <c r="V31" s="18"/>
-      <c r="W31" s="18"/>
-      <c r="X31" s="18"/>
-      <c r="Y31" s="21"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="21"/>
+      <c r="W31" s="21"/>
+      <c r="X31" s="21"/>
+      <c r="Y31" s="25"/>
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>87</v>
       </c>
-      <c r="H32" s="18"/>
-      <c r="I32" s="22" t="s">
+      <c r="H32" s="21"/>
+      <c r="I32" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="18"/>
-      <c r="X32" s="18"/>
-      <c r="Y32" s="21"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="21"/>
+      <c r="W32" s="21"/>
+      <c r="X32" s="21"/>
+      <c r="Y32" s="25"/>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>86</v>
       </c>
       <c r="C33" s="6"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="25" t="s">
+      <c r="H33" s="21"/>
+      <c r="I33" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
-      <c r="T33" s="18"/>
-      <c r="U33" s="18"/>
-      <c r="V33" s="18"/>
-      <c r="W33" s="18"/>
-      <c r="X33" s="18"/>
-      <c r="Y33" s="21"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="21"/>
+      <c r="Q33" s="21"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+      <c r="T33" s="21"/>
+      <c r="U33" s="21"/>
+      <c r="V33" s="21"/>
+      <c r="W33" s="21"/>
+      <c r="X33" s="21"/>
+      <c r="Y33" s="25"/>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>120</v>
       </c>
       <c r="C34" s="6"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="24" t="s">
+      <c r="H34" s="21"/>
+      <c r="I34" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
-      <c r="T34" s="18"/>
-      <c r="U34" s="18"/>
-      <c r="V34" s="18"/>
-      <c r="W34" s="18"/>
-      <c r="X34" s="18"/>
-      <c r="Y34" s="21"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="21"/>
+      <c r="Q34" s="21"/>
+      <c r="R34" s="21"/>
+      <c r="S34" s="21"/>
+      <c r="T34" s="21"/>
+      <c r="U34" s="21"/>
+      <c r="V34" s="21"/>
+      <c r="W34" s="21"/>
+      <c r="X34" s="21"/>
+      <c r="Y34" s="25"/>
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
@@ -3964,26 +3964,26 @@
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="23" t="s">
+      <c r="H35" s="21"/>
+      <c r="I35" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="18"/>
-      <c r="T35" s="18"/>
-      <c r="U35" s="18"/>
-      <c r="V35" s="18"/>
-      <c r="W35" s="18"/>
-      <c r="X35" s="18"/>
-      <c r="Y35" s="21"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="21"/>
+      <c r="Q35" s="21"/>
+      <c r="R35" s="21"/>
+      <c r="S35" s="21"/>
+      <c r="T35" s="21"/>
+      <c r="U35" s="21"/>
+      <c r="V35" s="21"/>
+      <c r="W35" s="21"/>
+      <c r="X35" s="21"/>
+      <c r="Y35" s="25"/>
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B36" s="6"/>
@@ -3992,26 +3992,26 @@
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="23" t="s">
+      <c r="H36" s="21"/>
+      <c r="I36" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="J36" s="23"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="18"/>
-      <c r="T36" s="18"/>
-      <c r="U36" s="18"/>
-      <c r="V36" s="18"/>
-      <c r="W36" s="18"/>
-      <c r="X36" s="18"/>
-      <c r="Y36" s="21"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
+      <c r="Q36" s="21"/>
+      <c r="R36" s="21"/>
+      <c r="S36" s="21"/>
+      <c r="T36" s="21"/>
+      <c r="U36" s="21"/>
+      <c r="V36" s="21"/>
+      <c r="W36" s="21"/>
+      <c r="X36" s="21"/>
+      <c r="Y36" s="25"/>
     </row>
     <row r="37" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
@@ -4020,26 +4020,26 @@
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="19" t="s">
+      <c r="H37" s="21"/>
+      <c r="I37" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
-      <c r="T37" s="18"/>
-      <c r="U37" s="18"/>
-      <c r="V37" s="18"/>
-      <c r="W37" s="18"/>
-      <c r="X37" s="18"/>
-      <c r="Y37" s="21"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="21"/>
+      <c r="R37" s="21"/>
+      <c r="S37" s="21"/>
+      <c r="T37" s="21"/>
+      <c r="U37" s="21"/>
+      <c r="V37" s="21"/>
+      <c r="W37" s="21"/>
+      <c r="X37" s="21"/>
+      <c r="Y37" s="25"/>
     </row>
     <row r="38" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
@@ -4048,26 +4048,26 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="23" t="s">
+      <c r="H38" s="21"/>
+      <c r="I38" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="J38" s="23"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
-      <c r="T38" s="18"/>
-      <c r="U38" s="18"/>
-      <c r="V38" s="18"/>
-      <c r="W38" s="18"/>
-      <c r="X38" s="18"/>
-      <c r="Y38" s="21"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="21"/>
+      <c r="R38" s="21"/>
+      <c r="S38" s="21"/>
+      <c r="T38" s="21"/>
+      <c r="U38" s="21"/>
+      <c r="V38" s="21"/>
+      <c r="W38" s="21"/>
+      <c r="X38" s="21"/>
+      <c r="Y38" s="25"/>
     </row>
     <row r="39" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
@@ -4076,26 +4076,26 @@
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="23" t="s">
+      <c r="H39" s="21"/>
+      <c r="I39" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="J39" s="23"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="18"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="18"/>
-      <c r="U39" s="18"/>
-      <c r="V39" s="18"/>
-      <c r="W39" s="18"/>
-      <c r="X39" s="18"/>
-      <c r="Y39" s="21"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="21"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="21"/>
+      <c r="T39" s="21"/>
+      <c r="U39" s="21"/>
+      <c r="V39" s="21"/>
+      <c r="W39" s="21"/>
+      <c r="X39" s="21"/>
+      <c r="Y39" s="25"/>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
@@ -4104,26 +4104,26 @@
         <v>11</v>
       </c>
       <c r="E40" s="6"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="23" t="s">
+      <c r="H40" s="21"/>
+      <c r="I40" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="J40" s="23"/>
-      <c r="K40" s="23"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="18"/>
-      <c r="U40" s="18"/>
-      <c r="V40" s="18"/>
-      <c r="W40" s="18"/>
-      <c r="X40" s="18"/>
-      <c r="Y40" s="21"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="21"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="21"/>
+      <c r="T40" s="21"/>
+      <c r="U40" s="21"/>
+      <c r="V40" s="21"/>
+      <c r="W40" s="21"/>
+      <c r="X40" s="21"/>
+      <c r="Y40" s="25"/>
     </row>
     <row r="41" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
@@ -4132,26 +4132,26 @@
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="19" t="s">
+      <c r="H41" s="21"/>
+      <c r="I41" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18"/>
-      <c r="O41" s="18"/>
-      <c r="P41" s="18"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
-      <c r="T41" s="18"/>
-      <c r="U41" s="18"/>
-      <c r="V41" s="18"/>
-      <c r="W41" s="18"/>
-      <c r="X41" s="18"/>
-      <c r="Y41" s="21"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="21"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="21"/>
+      <c r="T41" s="21"/>
+      <c r="U41" s="21"/>
+      <c r="V41" s="21"/>
+      <c r="W41" s="21"/>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="25"/>
     </row>
     <row r="42" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
@@ -4160,26 +4160,26 @@
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="23" t="s">
+      <c r="H42" s="21"/>
+      <c r="I42" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="J42" s="23"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
-      <c r="T42" s="18"/>
-      <c r="U42" s="18"/>
-      <c r="V42" s="18"/>
-      <c r="W42" s="18"/>
-      <c r="X42" s="18"/>
-      <c r="Y42" s="21"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="21"/>
+      <c r="Q42" s="21"/>
+      <c r="R42" s="21"/>
+      <c r="S42" s="21"/>
+      <c r="T42" s="21"/>
+      <c r="U42" s="21"/>
+      <c r="V42" s="21"/>
+      <c r="W42" s="21"/>
+      <c r="X42" s="21"/>
+      <c r="Y42" s="25"/>
     </row>
     <row r="43" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
@@ -4188,26 +4188,26 @@
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="23" t="s">
+      <c r="H43" s="21"/>
+      <c r="I43" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="J43" s="23"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
-      <c r="T43" s="18"/>
-      <c r="U43" s="18"/>
-      <c r="V43" s="18"/>
-      <c r="W43" s="18"/>
-      <c r="X43" s="18"/>
-      <c r="Y43" s="21"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
+      <c r="P43" s="21"/>
+      <c r="Q43" s="21"/>
+      <c r="R43" s="21"/>
+      <c r="S43" s="21"/>
+      <c r="T43" s="21"/>
+      <c r="U43" s="21"/>
+      <c r="V43" s="21"/>
+      <c r="W43" s="21"/>
+      <c r="X43" s="21"/>
+      <c r="Y43" s="25"/>
     </row>
     <row r="44" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
@@ -4216,26 +4216,26 @@
         <v>11</v>
       </c>
       <c r="E44" s="6"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="23" t="s">
+      <c r="H44" s="21"/>
+      <c r="I44" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J44" s="23"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="18"/>
-      <c r="U44" s="18"/>
-      <c r="V44" s="18"/>
-      <c r="W44" s="18"/>
-      <c r="X44" s="18"/>
-      <c r="Y44" s="21"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="21"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="21"/>
+      <c r="P44" s="21"/>
+      <c r="Q44" s="21"/>
+      <c r="R44" s="21"/>
+      <c r="S44" s="21"/>
+      <c r="T44" s="21"/>
+      <c r="U44" s="21"/>
+      <c r="V44" s="21"/>
+      <c r="W44" s="21"/>
+      <c r="X44" s="21"/>
+      <c r="Y44" s="25"/>
     </row>
     <row r="45" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
@@ -4244,26 +4244,26 @@
       <c r="E45" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H45" s="18"/>
-      <c r="I45" s="23" t="s">
+      <c r="H45" s="21"/>
+      <c r="I45" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J45" s="23"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="18"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
-      <c r="T45" s="18"/>
-      <c r="U45" s="18"/>
-      <c r="V45" s="18"/>
-      <c r="W45" s="18"/>
-      <c r="X45" s="18"/>
-      <c r="Y45" s="21"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="21"/>
+      <c r="P45" s="21"/>
+      <c r="Q45" s="21"/>
+      <c r="R45" s="21"/>
+      <c r="S45" s="21"/>
+      <c r="T45" s="21"/>
+      <c r="U45" s="21"/>
+      <c r="V45" s="21"/>
+      <c r="W45" s="21"/>
+      <c r="X45" s="21"/>
+      <c r="Y45" s="25"/>
     </row>
     <row r="46" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
@@ -4272,29 +4272,57 @@
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="19" t="s">
+      <c r="H46" s="21"/>
+      <c r="I46" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="18"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
-      <c r="T46" s="18"/>
-      <c r="U46" s="18"/>
-      <c r="V46" s="18"/>
-      <c r="W46" s="18"/>
-      <c r="X46" s="18"/>
-      <c r="Y46" s="21"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="21"/>
+      <c r="P46" s="21"/>
+      <c r="Q46" s="21"/>
+      <c r="R46" s="21"/>
+      <c r="S46" s="21"/>
+      <c r="T46" s="21"/>
+      <c r="U46" s="21"/>
+      <c r="V46" s="21"/>
+      <c r="W46" s="21"/>
+      <c r="X46" s="21"/>
+      <c r="Y46" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="H10:H46"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="J30:K30"/>
     <mergeCell ref="I34:K34"/>
     <mergeCell ref="Y10:Y46"/>
     <mergeCell ref="L10:X46"/>
@@ -4311,34 +4339,6 @@
     <mergeCell ref="I36:K36"/>
     <mergeCell ref="I37:K37"/>
     <mergeCell ref="I31:K31"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="H10:H46"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:J17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4350,7 +4350,7 @@
   <dimension ref="B2:Y21"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="I14" sqref="I14:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4380,28 +4380,28 @@
       <c r="H2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
       <c r="L2" s="9" t="s">
         <v>61</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20" t="s">
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
       <c r="U2" s="9" t="s">
         <v>65</v>
       </c>
@@ -4491,11 +4491,11 @@
       <c r="H9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
       <c r="L9" s="9" t="s">
         <v>95</v>
       </c>
@@ -4543,30 +4543,30 @@
       <c r="B10" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="18" t="s">
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="21" t="s">
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="25" t="s">
         <v>127</v>
       </c>
     </row>
@@ -4574,76 +4574,76 @@
       <c r="B11" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="23" t="s">
+      <c r="H11" s="21"/>
+      <c r="I11" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="21"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="21"/>
+      <c r="V11" s="21"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="25"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="23" t="s">
+      <c r="H12" s="21"/>
+      <c r="I12" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="18"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="21"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="25"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="23" t="s">
+      <c r="H13" s="21"/>
+      <c r="I13" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18"/>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="21"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="21"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="25"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -4652,219 +4652,212 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="23" t="s">
+      <c r="H14" s="21"/>
+      <c r="I14" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="Y14" s="21"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="21"/>
+      <c r="W14" s="21"/>
+      <c r="X14" s="21"/>
+      <c r="Y14" s="25"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="H15" s="18"/>
-      <c r="I15" s="22" t="s">
+      <c r="H15" s="21"/>
+      <c r="I15" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="18"/>
-      <c r="V15" s="18"/>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="21"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="21"/>
+      <c r="W15" s="21"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="25"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="22" t="s">
+      <c r="H16" s="21"/>
+      <c r="I16" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="21"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21"/>
+      <c r="V16" s="21"/>
+      <c r="W16" s="21"/>
+      <c r="X16" s="21"/>
+      <c r="Y16" s="25"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="H17" s="18"/>
-      <c r="I17" s="22" t="s">
+      <c r="H17" s="21"/>
+      <c r="I17" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="18"/>
-      <c r="V17" s="18"/>
-      <c r="W17" s="18"/>
-      <c r="X17" s="18"/>
-      <c r="Y17" s="21"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="21"/>
+      <c r="U17" s="21"/>
+      <c r="V17" s="21"/>
+      <c r="W17" s="21"/>
+      <c r="X17" s="21"/>
+      <c r="Y17" s="25"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="23" t="s">
+      <c r="H18" s="21"/>
+      <c r="I18" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="J18" s="19"/>
+      <c r="J18" s="18"/>
       <c r="K18" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="18"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="25"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="20" t="s">
+      <c r="H19" s="21"/>
+      <c r="I19" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="J19" s="20"/>
+      <c r="J19" s="23"/>
       <c r="K19" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="18"/>
-      <c r="U19" s="18"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="18"/>
-      <c r="X19" s="18"/>
-      <c r="Y19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="21"/>
+      <c r="W19" s="21"/>
+      <c r="X19" s="21"/>
+      <c r="Y19" s="25"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="18"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="J20" s="20" t="s">
+      <c r="J20" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="K20" s="20"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
-      <c r="T20" s="18"/>
-      <c r="U20" s="18"/>
-      <c r="V20" s="18"/>
-      <c r="W20" s="18"/>
-      <c r="X20" s="18"/>
-      <c r="Y20" s="21"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="21"/>
+      <c r="W20" s="21"/>
+      <c r="X20" s="21"/>
+      <c r="Y20" s="25"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="18"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="J21" s="25" t="s">
+      <c r="J21" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="K21" s="25"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
-      <c r="T21" s="18"/>
-      <c r="U21" s="18"/>
-      <c r="V21" s="18"/>
-      <c r="W21" s="18"/>
-      <c r="X21" s="18"/>
-      <c r="Y21" s="21"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="21"/>
+      <c r="V21" s="21"/>
+      <c r="W21" s="21"/>
+      <c r="X21" s="21"/>
+      <c r="Y21" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="Y10:Y21"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I19:J19"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
@@ -4877,6 +4870,13 @@
     <mergeCell ref="I12:K12"/>
     <mergeCell ref="I13:K13"/>
     <mergeCell ref="J21:K21"/>
+    <mergeCell ref="Y10:Y21"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I19:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4887,7 +4887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>